<commit_message>
experimental data for CGXII #5
</commit_message>
<xml_diff>
--- a/growth_binary/binary_growth_results.xlsx
+++ b/growth_binary/binary_growth_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/growth_binary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0684D7E5-21D5-FC4C-8002-3AE16A8A60F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479B4DDB-11D0-3147-B9AF-0FC0FC32E692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="LB" sheetId="5" r:id="rId3"/>
     <sheet name="CGXlab" sheetId="2" r:id="rId4"/>
     <sheet name="M9" sheetId="3" r:id="rId5"/>
-    <sheet name="CGXlab+" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
   <si>
     <t>strain</t>
   </si>
@@ -126,66 +125,17 @@
   <si>
     <t>CGXlab</t>
   </si>
-  <si>
-    <t>CGXII</t>
-  </si>
-  <si>
-    <t>CGXII+cobalt,pnto,cys__L</t>
-  </si>
-  <si>
-    <t>CGXII-ni,PCA,btn</t>
-  </si>
-  <si>
-    <t>CGXII-ni,PCA,btn+cobalt,pnto,cys__L</t>
-  </si>
-  <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>minimal</t>
-  </si>
-  <si>
-    <t>deprived</t>
-  </si>
-  <si>
-    <t>full</t>
-  </si>
-  <si>
-    <t>16-1</t>
-  </si>
-  <si>
-    <t>16-2</t>
-  </si>
-  <si>
-    <t>cobalt</t>
-  </si>
-  <si>
-    <t>0.013 g/L</t>
-  </si>
-  <si>
-    <t>pnto__R</t>
-  </si>
-  <si>
-    <t>0.001 g/L</t>
-  </si>
-  <si>
-    <t>cys__L</t>
-  </si>
-  <si>
-    <t>0.121 g/L</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000\ _$_-;\-* #,##0.000\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -252,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -293,7 +243,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -4785,7 +4734,7 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -6008,141 +5957,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA22BFD2-5EBD-4B47-B823-2C79A05C64D7}">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>0.155</v>
-      </c>
-      <c r="D2">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="E2">
-        <v>0.219</v>
-      </c>
-      <c r="F2" s="20">
-        <f>SUM(C2:E2)/3</f>
-        <v>0.18000000000000002</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3">
-        <v>0.224</v>
-      </c>
-      <c r="D3">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="E3">
-        <v>0.253</v>
-      </c>
-      <c r="F3" s="20">
-        <f t="shared" ref="F3:F5" si="0">SUM(C3:E3)/3</f>
-        <v>0.24666666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
-        <v>0.127</v>
-      </c>
-      <c r="D4">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="E4">
-        <v>0.125</v>
-      </c>
-      <c r="F4" s="20">
-        <f t="shared" si="0"/>
-        <v>0.13366666666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5">
-        <v>0.185</v>
-      </c>
-      <c r="D5">
-        <v>0.214</v>
-      </c>
-      <c r="E5">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="F5" s="20">
-        <f t="shared" si="0"/>
-        <v>0.20199999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>